<commit_message>
Update 3rd March 2025 2321 Hours
</commit_message>
<xml_diff>
--- a/Year 2025/DailyCodeCountYear2025.xlsx
+++ b/Year 2025/DailyCodeCountYear2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/180375e4ce017a01/Desktop/DailyCodeTracking/Year 2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="8_{5868F9CE-497B-4ABB-B43B-4F0C3C843604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF59EE8E-EC83-4054-B040-B1B5CBD847A0}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{5868F9CE-497B-4ABB-B43B-4F0C3C843604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37ABCF02-1AD5-4375-BDC7-179064057E15}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{853D40A3-D3A9-4D19-986B-DC8B7D1EBDCA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Month</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Spiral Matrix</t>
+  </si>
+  <si>
+    <t>Maximum Gap</t>
   </si>
 </sst>
 </file>
@@ -134,6 +137,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -433,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C4068F-A4DD-47AE-AC99-0E9EBFC91FAE}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -523,6 +530,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update [3rd March 2025 / (Today)] 2329 Hours
</commit_message>
<xml_diff>
--- a/Year 2025/DailyCodeCountYear2025.xlsx
+++ b/Year 2025/DailyCodeCountYear2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/180375e4ce017a01/Desktop/DailyCodeTracking/Year 2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="8_{5868F9CE-497B-4ABB-B43B-4F0C3C843604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37ABCF02-1AD5-4375-BDC7-179064057E15}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="8_{5868F9CE-497B-4ABB-B43B-4F0C3C843604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2F93F8B-B701-4CBA-97EC-291EE880BBFD}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{853D40A3-D3A9-4D19-986B-DC8B7D1EBDCA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Month</t>
   </si>
@@ -76,6 +76,24 @@
   </si>
   <si>
     <t>Maximum Gap</t>
+  </si>
+  <si>
+    <t>Maximum Subarray Sum</t>
+  </si>
+  <si>
+    <t>Maximum Product of Two Elements in an Array</t>
+  </si>
+  <si>
+    <t>Find N Unique Integers Sum up to Zero</t>
+  </si>
+  <si>
+    <t>Maximum Number of Pairs in Array</t>
+  </si>
+  <si>
+    <t>IntelliJ IDEA (PC)</t>
+  </si>
+  <si>
+    <t>Counting Sort</t>
   </si>
 </sst>
 </file>
@@ -440,16 +458,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C4068F-A4DD-47AE-AC99-0E9EBFC91FAE}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="6.3984375" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="3" max="3" width="38.59765625" customWidth="1"/>
     <col min="4" max="4" width="19.59765625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -527,15 +545,66 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
-        <v>6</v>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 4th March 2025 2353 Hours
</commit_message>
<xml_diff>
--- a/Year 2025/DailyCodeCountYear2025.xlsx
+++ b/Year 2025/DailyCodeCountYear2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/180375e4ce017a01/Desktop/DailyCodeTracking/Year 2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="8_{5868F9CE-497B-4ABB-B43B-4F0C3C843604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2F93F8B-B701-4CBA-97EC-291EE880BBFD}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{5868F9CE-497B-4ABB-B43B-4F0C3C843604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3980D53A-52F5-4552-94B9-84ECE4E4D1DD}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{853D40A3-D3A9-4D19-986B-DC8B7D1EBDCA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Month</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>Counting Sort</t>
+  </si>
+  <si>
+    <t>Count Negative Numbers in a Sorted Matrix</t>
+  </si>
+  <si>
+    <t>LeetCode</t>
+  </si>
+  <si>
+    <t>Squares of a Sorted Array</t>
   </si>
 </sst>
 </file>
@@ -458,17 +467,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C4068F-A4DD-47AE-AC99-0E9EBFC91FAE}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="6.3984375" customWidth="1"/>
     <col min="3" max="3" width="38.59765625" customWidth="1"/>
-    <col min="4" max="4" width="19.59765625" customWidth="1"/>
+    <col min="4" max="4" width="16.53125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
@@ -607,6 +616,25 @@
         <v>18</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update 5th March 2025 2344 Hours
</commit_message>
<xml_diff>
--- a/Year 2025/DailyCodeCountYear2025.xlsx
+++ b/Year 2025/DailyCodeCountYear2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/180375e4ce017a01/Desktop/DailyCodeTracking/Year 2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{5868F9CE-497B-4ABB-B43B-4F0C3C843604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3980D53A-52F5-4552-94B9-84ECE4E4D1DD}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="8_{5868F9CE-497B-4ABB-B43B-4F0C3C843604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B068F64-27D1-4665-BB13-8959F010E283}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{853D40A3-D3A9-4D19-986B-DC8B7D1EBDCA}"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{853D40A3-D3A9-4D19-986B-DC8B7D1EBDCA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>Month</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>Squares of a Sorted Array</t>
+  </si>
+  <si>
+    <t>Maximum Sum With Exactly K Elements</t>
+  </si>
+  <si>
+    <t>Richest Customer Wealth</t>
+  </si>
+  <si>
+    <t>1 to N (Recursion)</t>
   </si>
 </sst>
 </file>
@@ -467,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C4068F-A4DD-47AE-AC99-0E9EBFC91FAE}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -635,6 +644,33 @@
         <v>6</v>
       </c>
     </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update 7th March 2025 0012 Hours
</commit_message>
<xml_diff>
--- a/Year 2025/DailyCodeCountYear2025.xlsx
+++ b/Year 2025/DailyCodeCountYear2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/180375e4ce017a01/Desktop/DailyCodeTracking/Year 2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="8_{5868F9CE-497B-4ABB-B43B-4F0C3C843604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B068F64-27D1-4665-BB13-8959F010E283}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="8_{5868F9CE-497B-4ABB-B43B-4F0C3C843604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DF10EE7-B73C-4A02-BF3F-3F7FDA429270}"/>
   <bookViews>
-    <workbookView xWindow="28690" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{853D40A3-D3A9-4D19-986B-DC8B7D1EBDCA}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{853D40A3-D3A9-4D19-986B-DC8B7D1EBDCA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>Month</t>
   </si>
   <si>
-    <t>Problem Name</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -112,6 +109,18 @@
   </si>
   <si>
     <t>1 to N (Recursion)</t>
+  </si>
+  <si>
+    <t>Problem(s) Solved</t>
+  </si>
+  <si>
+    <t>Problem(s) Attempted</t>
+  </si>
+  <si>
+    <t>Elimination Game (Recursion)</t>
+  </si>
+  <si>
+    <t>Valid Sudoku</t>
   </si>
 </sst>
 </file>
@@ -476,199 +485,241 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C4068F-A4DD-47AE-AC99-0E9EBFC91FAE}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="6.3984375" customWidth="1"/>
     <col min="3" max="3" width="38.59765625" customWidth="1"/>
-    <col min="4" max="4" width="16.53125" customWidth="1"/>
+    <col min="4" max="4" width="35.19921875" customWidth="1"/>
+    <col min="5" max="5" width="17.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>3</v>
       </c>
       <c r="B2">
         <v>28</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C7" t="s">
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>3</v>
       </c>
       <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C11" t="s">
         <v>14</v>
       </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C11" t="s">
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C12" t="s">
         <v>15</v>
       </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C12" t="s">
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C13" t="s">
         <v>16</v>
       </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C13" t="s">
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
         <v>17</v>
       </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B15">
         <v>4</v>
       </c>
       <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
         <v>20</v>
       </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C16" t="s">
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
         <v>22</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B20">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B17">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" t="s">
-        <v>6</v>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 8th March 2025 2322 Hours
</commit_message>
<xml_diff>
--- a/Year 2025/DailyCodeCountYear2025.xlsx
+++ b/Year 2025/DailyCodeCountYear2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/180375e4ce017a01/Desktop/DailyCodeTracking/Year 2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="8_{5868F9CE-497B-4ABB-B43B-4F0C3C843604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DF10EE7-B73C-4A02-BF3F-3F7FDA429270}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="8_{5868F9CE-497B-4ABB-B43B-4F0C3C843604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EED5431B-4DD6-4754-BADF-D10F4DDA7503}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{853D40A3-D3A9-4D19-986B-DC8B7D1EBDCA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>Month</t>
   </si>
@@ -121,6 +121,15 @@
   </si>
   <si>
     <t>Valid Sudoku</t>
+  </si>
+  <si>
+    <t>Rotate Image</t>
+  </si>
+  <si>
+    <t>Flipping an Image</t>
+  </si>
+  <si>
+    <t>Set Matrix Zero</t>
   </si>
 </sst>
 </file>
@@ -485,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C4068F-A4DD-47AE-AC99-0E9EBFC91FAE}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -722,6 +731,33 @@
         <v>20</v>
       </c>
     </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update 9th March 2025 2341 Hours
</commit_message>
<xml_diff>
--- a/Year 2025/DailyCodeCountYear2025.xlsx
+++ b/Year 2025/DailyCodeCountYear2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/180375e4ce017a01/Desktop/DailyCodeTracking/Year 2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="121" documentId="8_{5868F9CE-497B-4ABB-B43B-4F0C3C843604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EED5431B-4DD6-4754-BADF-D10F4DDA7503}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="8_{5868F9CE-497B-4ABB-B43B-4F0C3C843604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32D82E01-DE03-4EC7-A91A-0A55EFB61834}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{853D40A3-D3A9-4D19-986B-DC8B7D1EBDCA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
   <si>
     <t>Month</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Set Matrix Zero</t>
+  </si>
+  <si>
+    <t>Reshape the Matrix</t>
   </si>
 </sst>
 </file>
@@ -494,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C4068F-A4DD-47AE-AC99-0E9EBFC91FAE}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -758,6 +761,17 @@
         <v>20</v>
       </c>
     </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B27">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update 11th March 2025 0105 Hours
</commit_message>
<xml_diff>
--- a/Year 2025/DailyCodeCountYear2025.xlsx
+++ b/Year 2025/DailyCodeCountYear2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/180375e4ce017a01/Desktop/DailyCodeTracking/Year 2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="8_{5868F9CE-497B-4ABB-B43B-4F0C3C843604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32D82E01-DE03-4EC7-A91A-0A55EFB61834}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="8_{5868F9CE-497B-4ABB-B43B-4F0C3C843604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A476DBB-CB3A-449A-89B7-4501044B5683}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{853D40A3-D3A9-4D19-986B-DC8B7D1EBDCA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
   <si>
     <t>Month</t>
   </si>
@@ -133,6 +133,15 @@
   </si>
   <si>
     <t>Reshape the Matrix</t>
+  </si>
+  <si>
+    <t>Rotate Image 2</t>
+  </si>
+  <si>
+    <t>FillMatrixByRecursion</t>
+  </si>
+  <si>
+    <t>PermutationsOfAString</t>
   </si>
 </sst>
 </file>
@@ -497,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C4068F-A4DD-47AE-AC99-0E9EBFC91FAE}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -742,34 +751,69 @@
         <v>29</v>
       </c>
       <c r="E24" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C25" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E25" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E26" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B27">
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C28" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B29">
         <v>9</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C29" t="s">
         <v>32</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E29" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 12th March 2025 2335 Hours
</commit_message>
<xml_diff>
--- a/Year 2025/DailyCodeCountYear2025.xlsx
+++ b/Year 2025/DailyCodeCountYear2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/180375e4ce017a01/Desktop/DailyCodeTracking/Year 2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="8_{5868F9CE-497B-4ABB-B43B-4F0C3C843604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A476DBB-CB3A-449A-89B7-4501044B5683}"/>
+  <xr:revisionPtr revIDLastSave="172" documentId="8_{5868F9CE-497B-4ABB-B43B-4F0C3C843604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85F61F41-D7E6-4246-942E-FBCDBB81C99B}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{853D40A3-D3A9-4D19-986B-DC8B7D1EBDCA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
   <si>
     <t>Month</t>
   </si>
@@ -123,25 +123,46 @@
     <t>Valid Sudoku</t>
   </si>
   <si>
-    <t>Rotate Image</t>
-  </si>
-  <si>
     <t>Flipping an Image</t>
   </si>
   <si>
-    <t>Set Matrix Zero</t>
-  </si>
-  <si>
     <t>Reshape the Matrix</t>
   </si>
   <si>
-    <t>Rotate Image 2</t>
-  </si>
-  <si>
     <t>FillMatrixByRecursion</t>
   </si>
   <si>
     <t>PermutationsOfAString</t>
+  </si>
+  <si>
+    <t>RotateImage</t>
+  </si>
+  <si>
+    <t>RotateImage2</t>
+  </si>
+  <si>
+    <t>Set Matrix Zero (Solution 1)</t>
+  </si>
+  <si>
+    <t>Set Matrix Zero (Solution 2)</t>
+  </si>
+  <si>
+    <t>SubsetsOfAString</t>
+  </si>
+  <si>
+    <t>Subsets (Solution 1)</t>
+  </si>
+  <si>
+    <t>Subsets (Solution 2)</t>
+  </si>
+  <si>
+    <t>Permutations</t>
+  </si>
+  <si>
+    <t>Rotate Image (Solution 1)</t>
+  </si>
+  <si>
+    <t>Rotate Image (Solution 2)</t>
   </si>
 </sst>
 </file>
@@ -506,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C4068F-A4DD-47AE-AC99-0E9EBFC91FAE}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -748,7 +769,7 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E24" t="s">
         <v>17</v>
@@ -756,7 +777,7 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E25" t="s">
         <v>17</v>
@@ -764,7 +785,7 @@
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C26" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="E26" t="s">
         <v>20</v>
@@ -772,26 +793,23 @@
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C27" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="E27" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C28" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E28" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B29">
-        <v>9</v>
-      </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E29" t="s">
         <v>20</v>
@@ -799,21 +817,91 @@
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B30">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E30" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C31" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C33" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B34">
+        <v>11</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C36" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B37">
+        <v>12</v>
+      </c>
+      <c r="C37" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C38" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B39">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 15th March 2025 2328 Hours
</commit_message>
<xml_diff>
--- a/Year 2025/DailyCodeCountYear2025.xlsx
+++ b/Year 2025/DailyCodeCountYear2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/180375e4ce017a01/Desktop/DailyCodeTracking/Year 2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="172" documentId="8_{5868F9CE-497B-4ABB-B43B-4F0C3C843604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85F61F41-D7E6-4246-942E-FBCDBB81C99B}"/>
+  <xr:revisionPtr revIDLastSave="195" documentId="8_{5868F9CE-497B-4ABB-B43B-4F0C3C843604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E82AAB28-9E37-44E0-8678-34E70D5FBA37}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{853D40A3-D3A9-4D19-986B-DC8B7D1EBDCA}"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{853D40A3-D3A9-4D19-986B-DC8B7D1EBDCA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="51">
   <si>
     <t>Month</t>
   </si>
@@ -163,6 +163,30 @@
   </si>
   <si>
     <t>Rotate Image (Solution 2)</t>
+  </si>
+  <si>
+    <t>Permutations II</t>
+  </si>
+  <si>
+    <t>Subsets II</t>
+  </si>
+  <si>
+    <t>Leetcode</t>
+  </si>
+  <si>
+    <t>Combination Sum (Solution 1)</t>
+  </si>
+  <si>
+    <t>Combination Sum II (Solution 1)</t>
+  </si>
+  <si>
+    <t>Count of Smaller Numbers After Self</t>
+  </si>
+  <si>
+    <t>Combination Sum (Solution 2)</t>
+  </si>
+  <si>
+    <t>Merge Sorted Array</t>
   </si>
 </sst>
 </file>
@@ -527,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C4068F-A4DD-47AE-AC99-0E9EBFC91FAE}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -903,6 +927,74 @@
       <c r="B39">
         <v>13</v>
       </c>
+      <c r="C39" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C40" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C42" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C43" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B44">
+        <v>14</v>
+      </c>
+      <c r="C44" t="s">
+        <v>48</v>
+      </c>
+      <c r="E44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B45">
+        <v>15</v>
+      </c>
+      <c r="C45" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C46" t="s">
+        <v>50</v>
+      </c>
+      <c r="E46" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>